<commit_message>
# Apply the pattern fill to the entire sheet for row in sheet.iter_rows():     for cell in row:         cell.fill = pattern_fill
</commit_message>
<xml_diff>
--- a/Customers Bills/main_sheet.xlsx
+++ b/Customers Bills/main_sheet.xlsx
@@ -29,24 +29,12 @@
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00ADD8E6"/>
-        <bgColor rgb="00ADD8E6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FFFFFF"/>
-        <bgColor rgb="00FFFFFF"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -64,8 +52,12 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -431,7 +423,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -439,9 +431,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="7.199999999999999" customWidth="1" min="1" max="1"/>
-    <col width="7.199999999999999" customWidth="1" min="2" max="2"/>
-    <col width="13.2" customWidth="1" min="3" max="3"/>
+    <col width="12" customWidth="1" min="1" max="1"/>
+    <col width="12" customWidth="1" min="2" max="2"/>
+    <col width="16.8" customWidth="1" min="3" max="3"/>
     <col width="21.6" customWidth="1" min="4" max="4"/>
     <col width="30" customWidth="1" min="5" max="5"/>
     <col width="16.8" customWidth="1" min="6" max="6"/>
@@ -450,164 +442,562 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>Time</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>Unique ID</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>Transaction Type</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t>Transaction Description</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" s="2" t="inlineStr">
         <is>
           <t>Amount (EGP)</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Notes</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="G1" s="2" t="inlineStr">
+        <is>
+          <t>Notes</t>
+        </is>
+      </c>
+      <c r="H1" s="2" t="inlineStr">
         <is>
           <t>Logged by:</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="n"/>
-      <c r="B2" s="2" t="n"/>
-      <c r="C2" s="2" t="n"/>
-      <c r="D2" s="2" t="n"/>
+      <c r="A2" s="3" t="inlineStr">
+        <is>
+          <t>15/06/24</t>
+        </is>
+      </c>
+      <c r="B2" s="3" t="inlineStr">
+        <is>
+          <t>17:55:13</t>
+        </is>
+      </c>
+      <c r="C2" s="3" t="inlineStr">
+        <is>
+          <t>150624175513</t>
+        </is>
+      </c>
+      <c r="D2" s="3" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="E2" s="3" t="inlineStr">
+        <is>
+          <t>Yara Mahmoud's Bill</t>
+        </is>
+      </c>
+      <c r="F2" s="3" t="n">
+        <v>800</v>
+      </c>
+      <c r="G2" s="3" t="inlineStr">
+        <is>
+          <t>Notes</t>
+        </is>
+      </c>
+      <c r="H2" s="3" t="inlineStr">
+        <is>
+          <t>asdas</t>
+        </is>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="n"/>
-      <c r="B3" s="3" t="n"/>
-      <c r="C3" s="3" t="n"/>
-      <c r="D3" s="3" t="n"/>
+      <c r="A3" s="3" t="inlineStr">
+        <is>
+          <t>15/06/24</t>
+        </is>
+      </c>
+      <c r="B3" s="3" t="inlineStr">
+        <is>
+          <t>17:56:31</t>
+        </is>
+      </c>
+      <c r="C3" s="3" t="inlineStr">
+        <is>
+          <t>150624175631</t>
+        </is>
+      </c>
+      <c r="D3" s="3" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="E3" s="3" t="inlineStr">
+        <is>
+          <t>Yara Mahmoud's Bill</t>
+        </is>
+      </c>
+      <c r="F3" s="3" t="n">
+        <v>800</v>
+      </c>
+      <c r="G3" s="3" t="inlineStr">
+        <is>
+          <t>Notes</t>
+        </is>
+      </c>
+      <c r="H3" s="3" t="inlineStr">
+        <is>
+          <t>asdas</t>
+        </is>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="n"/>
-      <c r="B4" s="2" t="n"/>
-      <c r="C4" s="2" t="n"/>
-      <c r="D4" s="2" t="n"/>
+      <c r="A4" s="3" t="inlineStr">
+        <is>
+          <t>15/06/24</t>
+        </is>
+      </c>
+      <c r="B4" s="3" t="inlineStr">
+        <is>
+          <t>17:56:35</t>
+        </is>
+      </c>
+      <c r="C4" s="3" t="inlineStr">
+        <is>
+          <t>150624175635</t>
+        </is>
+      </c>
+      <c r="D4" s="3" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="E4" s="3" t="inlineStr">
+        <is>
+          <t>Yara Mahmoud's Bill</t>
+        </is>
+      </c>
+      <c r="F4" s="3" t="n">
+        <v>800</v>
+      </c>
+      <c r="G4" s="3" t="inlineStr">
+        <is>
+          <t>Notes</t>
+        </is>
+      </c>
+      <c r="H4" s="3" t="inlineStr">
+        <is>
+          <t>asdas</t>
+        </is>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" s="3" t="n"/>
-      <c r="B5" s="3" t="n"/>
-      <c r="C5" s="3" t="n"/>
-      <c r="D5" s="3" t="n"/>
+      <c r="A5" s="3" t="inlineStr">
+        <is>
+          <t>15/06/24</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="inlineStr">
+        <is>
+          <t>17:57:26</t>
+        </is>
+      </c>
+      <c r="C5" s="3" t="inlineStr">
+        <is>
+          <t>150624175726</t>
+        </is>
+      </c>
+      <c r="D5" s="3" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="E5" s="3" t="inlineStr">
+        <is>
+          <t>Yara Mahmoud's Bill</t>
+        </is>
+      </c>
+      <c r="F5" s="3" t="n">
+        <v>1600</v>
+      </c>
+      <c r="G5" s="3" t="inlineStr">
+        <is>
+          <t>Notes</t>
+        </is>
+      </c>
+      <c r="H5" s="3" t="inlineStr">
+        <is>
+          <t>asdas</t>
+        </is>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" s="2" t="n"/>
-      <c r="B6" s="2" t="n"/>
-      <c r="C6" s="2" t="n"/>
-      <c r="D6" s="2" t="n"/>
+      <c r="A6" s="3" t="inlineStr">
+        <is>
+          <t>15/06/24</t>
+        </is>
+      </c>
+      <c r="B6" s="3" t="inlineStr">
+        <is>
+          <t>17:58:00</t>
+        </is>
+      </c>
+      <c r="C6" s="3" t="inlineStr">
+        <is>
+          <t>150624175800</t>
+        </is>
+      </c>
+      <c r="D6" s="3" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="E6" s="3" t="inlineStr">
+        <is>
+          <t>Yara Mahmoud's Bill</t>
+        </is>
+      </c>
+      <c r="F6" s="3" t="n">
+        <v>1340</v>
+      </c>
+      <c r="G6" s="3" t="inlineStr">
+        <is>
+          <t>Notes</t>
+        </is>
+      </c>
+      <c r="H6" s="3" t="inlineStr">
+        <is>
+          <t>asdas</t>
+        </is>
+      </c>
     </row>
     <row r="7">
-      <c r="A7" s="3" t="n"/>
-      <c r="B7" s="3" t="n"/>
-      <c r="C7" s="3" t="n"/>
-      <c r="D7" s="3" t="n"/>
+      <c r="A7" s="3" t="inlineStr">
+        <is>
+          <t>15/06/24</t>
+        </is>
+      </c>
+      <c r="B7" s="3" t="inlineStr">
+        <is>
+          <t>17:58:04</t>
+        </is>
+      </c>
+      <c r="C7" s="3" t="inlineStr">
+        <is>
+          <t>150624175804</t>
+        </is>
+      </c>
+      <c r="D7" s="3" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="E7" s="3" t="inlineStr">
+        <is>
+          <t>Yara Mahmoud's Bill</t>
+        </is>
+      </c>
+      <c r="F7" s="3" t="n">
+        <v>1340</v>
+      </c>
+      <c r="G7" s="3" t="inlineStr">
+        <is>
+          <t>Notes</t>
+        </is>
+      </c>
+      <c r="H7" s="3" t="inlineStr">
+        <is>
+          <t>asdas</t>
+        </is>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" s="2" t="n"/>
-      <c r="B8" s="2" t="n"/>
-      <c r="C8" s="2" t="n"/>
-      <c r="D8" s="2" t="n"/>
+      <c r="A8" s="3" t="inlineStr">
+        <is>
+          <t>15/06/24</t>
+        </is>
+      </c>
+      <c r="B8" s="3" t="inlineStr">
+        <is>
+          <t>17:58:08</t>
+        </is>
+      </c>
+      <c r="C8" s="3" t="inlineStr">
+        <is>
+          <t>150624175808</t>
+        </is>
+      </c>
+      <c r="D8" s="3" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="E8" s="3" t="inlineStr">
+        <is>
+          <t>Yara Mahmoud's Bill</t>
+        </is>
+      </c>
+      <c r="F8" s="3" t="n">
+        <v>1340</v>
+      </c>
+      <c r="G8" s="3" t="inlineStr">
+        <is>
+          <t>Notes</t>
+        </is>
+      </c>
+      <c r="H8" s="3" t="inlineStr">
+        <is>
+          <t>asdas</t>
+        </is>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>15/06/24</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>16:46</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>1506241646</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>IN</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>Sara Ibrahim's Bill</t>
-        </is>
-      </c>
-      <c r="F9" t="n">
-        <v>330</v>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>Notes</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
+      <c r="A9" s="3" t="inlineStr">
+        <is>
+          <t>15/06/24</t>
+        </is>
+      </c>
+      <c r="B9" s="3" t="inlineStr">
+        <is>
+          <t>17:58:10</t>
+        </is>
+      </c>
+      <c r="C9" s="3" t="inlineStr">
+        <is>
+          <t>150624175810</t>
+        </is>
+      </c>
+      <c r="D9" s="3" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="E9" s="3" t="inlineStr">
+        <is>
+          <t>Yara Mahmoud's Bill</t>
+        </is>
+      </c>
+      <c r="F9" s="3" t="n">
+        <v>1340</v>
+      </c>
+      <c r="G9" s="3" t="inlineStr">
+        <is>
+          <t>Notes</t>
+        </is>
+      </c>
+      <c r="H9" s="3" t="inlineStr">
         <is>
           <t>asdas</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>15/06/24</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>16:47</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>1506241647</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>IN</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>NEW TEST's Bill</t>
-        </is>
-      </c>
-      <c r="F10" t="n">
-        <v>800</v>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>Notes</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
+      <c r="A10" s="3" t="inlineStr">
+        <is>
+          <t>15/06/24</t>
+        </is>
+      </c>
+      <c r="B10" s="3" t="inlineStr">
+        <is>
+          <t>17:58:13</t>
+        </is>
+      </c>
+      <c r="C10" s="3" t="inlineStr">
+        <is>
+          <t>150624175813</t>
+        </is>
+      </c>
+      <c r="D10" s="3" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="E10" s="3" t="inlineStr">
+        <is>
+          <t>Yara Mahmoud's Bill</t>
+        </is>
+      </c>
+      <c r="F10" s="3" t="n">
+        <v>1340</v>
+      </c>
+      <c r="G10" s="3" t="inlineStr">
+        <is>
+          <t>Notes</t>
+        </is>
+      </c>
+      <c r="H10" s="3" t="inlineStr">
+        <is>
+          <t>asdas</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="3" t="inlineStr">
+        <is>
+          <t>15/06/24</t>
+        </is>
+      </c>
+      <c r="B11" s="3" t="inlineStr">
+        <is>
+          <t>17:58:44</t>
+        </is>
+      </c>
+      <c r="C11" s="3" t="inlineStr">
+        <is>
+          <t>150624175844</t>
+        </is>
+      </c>
+      <c r="D11" s="3" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="E11" s="3" t="inlineStr">
+        <is>
+          <t>Yara Mahmoud's Bill</t>
+        </is>
+      </c>
+      <c r="F11" s="3" t="n">
+        <v>990</v>
+      </c>
+      <c r="G11" s="3" t="inlineStr">
+        <is>
+          <t>Notes</t>
+        </is>
+      </c>
+      <c r="H11" s="3" t="inlineStr">
+        <is>
+          <t>asdas</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="3" t="inlineStr">
+        <is>
+          <t>15/06/24</t>
+        </is>
+      </c>
+      <c r="B12" s="3" t="inlineStr">
+        <is>
+          <t>18:00:34</t>
+        </is>
+      </c>
+      <c r="C12" s="3" t="inlineStr">
+        <is>
+          <t>150624180034</t>
+        </is>
+      </c>
+      <c r="D12" s="3" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="E12" s="3" t="inlineStr">
+        <is>
+          <t>Yara Mahmoud's Bill</t>
+        </is>
+      </c>
+      <c r="F12" s="3" t="n">
+        <v>370</v>
+      </c>
+      <c r="G12" s="3" t="inlineStr">
+        <is>
+          <t>Notes</t>
+        </is>
+      </c>
+      <c r="H12" s="3" t="inlineStr">
+        <is>
+          <t>asdas</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="3" t="inlineStr">
+        <is>
+          <t>15/06/24</t>
+        </is>
+      </c>
+      <c r="B13" s="3" t="inlineStr">
+        <is>
+          <t>18:01:07</t>
+        </is>
+      </c>
+      <c r="C13" s="3" t="inlineStr">
+        <is>
+          <t>150624180107</t>
+        </is>
+      </c>
+      <c r="D13" s="3" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="E13" s="3" t="inlineStr">
+        <is>
+          <t>Yara Mahmoud's Bill</t>
+        </is>
+      </c>
+      <c r="F13" s="3" t="n">
+        <v>1150</v>
+      </c>
+      <c r="G13" s="3" t="inlineStr">
+        <is>
+          <t>Notes</t>
+        </is>
+      </c>
+      <c r="H13" s="3" t="inlineStr">
+        <is>
+          <t>asdas</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>15/06/24</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>18:01:11</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>150624180111</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Yara Mahmoud's Bill</t>
+        </is>
+      </c>
+      <c r="F14" t="n">
+        <v>1150</v>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Notes</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
         <is>
           <t>asdas</t>
         </is>

</xml_diff>